<commit_message>
metrics by room work
</commit_message>
<xml_diff>
--- a/all_metrics.xlsx
+++ b/all_metrics.xlsx
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45755.46653729503</v>
+        <v>45755.49761152277</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45755.46653782742</v>
+        <v>45755.49761203125</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45755.46653836523</v>
+        <v>45755.4976125281</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -641,7 +641,7 @@
         </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45755.46653886374</v>
+        <v>45755.49761298736</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45755.46653936864</v>
+        <v>45755.49761345738</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -734,7 +734,7 @@
         </is>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45755.46653989011</v>
+        <v>45755.49761392974</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45755.46654039645</v>
+        <v>45755.49761439126</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45755.46654095147</v>
+        <v>45755.49761489518</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -863,7 +863,7 @@
         </is>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45755.46654150802</v>
+        <v>45755.49761539219</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -906,7 +906,7 @@
         </is>
       </c>
       <c r="F11" s="2" t="n">
-        <v>45755.46654202377</v>
+        <v>45755.49761587066</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="F12" s="2" t="n">
-        <v>45755.46654254476</v>
+        <v>45755.49761635419</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="F13" s="2" t="n">
-        <v>45755.4665430907</v>
+        <v>45755.49761684499</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1035,7 +1035,7 @@
         </is>
       </c>
       <c r="F14" s="2" t="n">
-        <v>45755.46654367878</v>
+        <v>45755.49761733141</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="F15" s="2" t="n">
-        <v>45755.4665442492</v>
+        <v>45755.49761778831</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="F16" s="2" t="n">
-        <v>45755.46654476658</v>
+        <v>45755.49761824885</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
         </is>
       </c>
       <c r="F17" s="2" t="n">
-        <v>45755.46654523908</v>
+        <v>45755.49761870743</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="F18" s="2" t="n">
-        <v>45755.4665457001</v>
+        <v>45755.49761916386</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="F19" s="2" t="n">
-        <v>45755.466546164</v>
+        <v>45755.49761963147</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="F20" s="2" t="n">
-        <v>45755.46654663033</v>
+        <v>45755.49762010983</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         </is>
       </c>
       <c r="F21" s="2" t="n">
-        <v>45755.46654713761</v>
+        <v>45755.49762063603</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1379,7 +1379,7 @@
         </is>
       </c>
       <c r="F22" s="2" t="n">
-        <v>45755.46654769236</v>
+        <v>45755.49762121544</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="F23" s="2" t="n">
-        <v>45755.46654831542</v>
+        <v>45755.49762183748</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="F24" s="2" t="n">
-        <v>45755.4665489668</v>
+        <v>45755.49762243995</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1508,7 +1508,7 @@
         </is>
       </c>
       <c r="F25" s="2" t="n">
-        <v>45755.46654975095</v>
+        <v>45755.4976231757</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1551,7 +1551,7 @@
         </is>
       </c>
       <c r="F26" s="2" t="n">
-        <v>45755.46655053529</v>
+        <v>45755.49762400453</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1594,7 +1594,7 @@
         </is>
       </c>
       <c r="F27" s="2" t="n">
-        <v>45755.46655130038</v>
+        <v>45755.49762476129</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1637,7 +1637,7 @@
         </is>
       </c>
       <c r="F28" s="2" t="n">
-        <v>45755.46655192121</v>
+        <v>45755.49762540319</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1680,7 +1680,7 @@
         </is>
       </c>
       <c r="F29" s="2" t="n">
-        <v>45755.46655264543</v>
+        <v>45755.49762615035</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1723,7 +1723,7 @@
         </is>
       </c>
       <c r="F30" s="2" t="n">
-        <v>45755.46655337461</v>
+        <v>45755.49762688735</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1766,7 +1766,7 @@
         </is>
       </c>
       <c r="F31" s="2" t="n">
-        <v>45755.46655401301</v>
+        <v>45755.49762754246</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="F32" s="2" t="n">
-        <v>45755.46655449427</v>
+        <v>45755.49762804621</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1855,7 +1855,7 @@
         </is>
       </c>
       <c r="F33" s="2" t="n">
-        <v>45755.46655501516</v>
+        <v>45755.49762854267</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1898,7 +1898,7 @@
         </is>
       </c>
       <c r="F34" s="2" t="n">
-        <v>45755.46655556717</v>
+        <v>45755.49762904022</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1941,7 +1941,7 @@
         </is>
       </c>
       <c r="F35" s="2" t="n">
-        <v>45755.46655611493</v>
+        <v>45755.49762953878</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1984,7 +1984,7 @@
         </is>
       </c>
       <c r="F36" s="2" t="n">
-        <v>45755.46655665732</v>
+        <v>45755.49763002522</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2027,7 +2027,7 @@
         </is>
       </c>
       <c r="F37" s="2" t="n">
-        <v>45755.46655716548</v>
+        <v>45755.49763052198</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -2070,7 +2070,7 @@
         </is>
       </c>
       <c r="F38" s="2" t="n">
-        <v>45755.46655765022</v>
+        <v>45755.49763101414</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -2118,7 +2118,7 @@
         </is>
       </c>
       <c r="F39" s="2" t="n">
-        <v>45755.46655811774</v>
+        <v>45755.49763151296</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -2161,7 +2161,7 @@
         </is>
       </c>
       <c r="F40" s="2" t="n">
-        <v>45755.46655859528</v>
+        <v>45755.49763204808</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -2204,7 +2204,7 @@
         </is>
       </c>
       <c r="F41" s="2" t="n">
-        <v>45755.46655906943</v>
+        <v>45755.49763260873</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -2247,7 +2247,7 @@
         </is>
       </c>
       <c r="F42" s="2" t="n">
-        <v>45755.4665595382</v>
+        <v>45755.49763314609</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -2290,7 +2290,7 @@
         </is>
       </c>
       <c r="F43" s="2" t="n">
-        <v>45755.46656002318</v>
+        <v>45755.49763368889</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -2333,7 +2333,7 @@
         </is>
       </c>
       <c r="F44" s="2" t="n">
-        <v>45755.46656051735</v>
+        <v>45755.49763424006</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -2376,7 +2376,7 @@
         </is>
       </c>
       <c r="F45" s="2" t="n">
-        <v>45755.46656105801</v>
+        <v>45755.49763484202</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -2419,7 +2419,7 @@
         </is>
       </c>
       <c r="F46" s="2" t="n">
-        <v>45755.46656173082</v>
+        <v>45755.49763542184</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2462,7 +2462,7 @@
         </is>
       </c>
       <c r="F47" s="2" t="n">
-        <v>45755.46656231004</v>
+        <v>45755.49763597224</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2505,7 +2505,7 @@
         </is>
       </c>
       <c r="F48" s="2" t="n">
-        <v>45755.46656284841</v>
+        <v>45755.49763651122</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2548,7 +2548,7 @@
         </is>
       </c>
       <c r="F49" s="2" t="n">
-        <v>45755.46656344367</v>
+        <v>45755.49763712604</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2591,7 +2591,7 @@
         </is>
       </c>
       <c r="F50" s="2" t="n">
-        <v>45755.46656412044</v>
+        <v>45755.49763779818</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2634,7 +2634,7 @@
         </is>
       </c>
       <c r="F51" s="2" t="n">
-        <v>45755.46656473819</v>
+        <v>45755.4976384814</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2677,7 +2677,7 @@
         </is>
       </c>
       <c r="F52" s="2" t="n">
-        <v>45755.46656532206</v>
+        <v>45755.49763912116</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2724,7 +2724,7 @@
         </is>
       </c>
       <c r="F53" s="2" t="n">
-        <v>45755.46656592075</v>
+        <v>45755.49763976256</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2771,7 +2771,7 @@
         </is>
       </c>
       <c r="F54" s="2" t="n">
-        <v>45755.46656654312</v>
+        <v>45755.4976404122</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2814,7 +2814,7 @@
         </is>
       </c>
       <c r="F55" s="2" t="n">
-        <v>45755.46656709273</v>
+        <v>45755.49764094692</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2857,7 +2857,7 @@
         </is>
       </c>
       <c r="F56" s="2" t="n">
-        <v>45755.4665676747</v>
+        <v>45755.4976415287</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -2900,7 +2900,7 @@
         </is>
       </c>
       <c r="F57" s="2" t="n">
-        <v>45755.46656821032</v>
+        <v>45755.49764206883</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2943,7 +2943,7 @@
         </is>
       </c>
       <c r="F58" s="2" t="n">
-        <v>45755.46656839186</v>
+        <v>45755.49764226161</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="F59" s="2" t="n">
-        <v>45755.46656841462</v>
+        <v>45755.49764228757</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -3029,7 +3029,7 @@
         </is>
       </c>
       <c r="F60" s="2" t="n">
-        <v>45755.46656843889</v>
+        <v>45755.49764231433</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -3072,7 +3072,7 @@
         </is>
       </c>
       <c r="F61" s="2" t="n">
-        <v>45755.46656846472</v>
+        <v>45755.497642341</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -3115,7 +3115,7 @@
         </is>
       </c>
       <c r="F62" s="2" t="n">
-        <v>45755.4665684905</v>
+        <v>45755.49764236955</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -3158,7 +3158,7 @@
         </is>
       </c>
       <c r="F63" s="2" t="n">
-        <v>45755.46656850978</v>
+        <v>45755.49764239001</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -3201,7 +3201,7 @@
         </is>
       </c>
       <c r="F64" s="2" t="n">
-        <v>45755.46656853182</v>
+        <v>45755.4976424116</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -3244,7 +3244,7 @@
         </is>
       </c>
       <c r="F65" s="2" t="n">
-        <v>45755.46656855672</v>
+        <v>45755.49764243234</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -3287,7 +3287,7 @@
         </is>
       </c>
       <c r="F66" s="2" t="n">
-        <v>45755.46656857616</v>
+        <v>45755.49764245288</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -3330,7 +3330,7 @@
         </is>
       </c>
       <c r="F67" s="2" t="n">
-        <v>45755.46656859655</v>
+        <v>45755.49764247286</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -3373,7 +3373,7 @@
         </is>
       </c>
       <c r="F68" s="2" t="n">
-        <v>45755.46656861559</v>
+        <v>45755.49764249208</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -3416,7 +3416,7 @@
         </is>
       </c>
       <c r="F69" s="2" t="n">
-        <v>45755.46656863809</v>
+        <v>45755.49764251693</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -3459,7 +3459,7 @@
         </is>
       </c>
       <c r="F70" s="2" t="n">
-        <v>45755.46656865961</v>
+        <v>45755.49764253719</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -3502,7 +3502,7 @@
         </is>
       </c>
       <c r="F71" s="2" t="n">
-        <v>45755.46656868055</v>
+        <v>45755.49764255891</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -3545,7 +3545,7 @@
         </is>
       </c>
       <c r="F72" s="2" t="n">
-        <v>45755.46656869897</v>
+        <v>45755.49764257762</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -3588,7 +3588,7 @@
         </is>
       </c>
       <c r="F73" s="2" t="n">
-        <v>45755.46656871762</v>
+        <v>45755.49764260096</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -3631,7 +3631,7 @@
         </is>
       </c>
       <c r="F74" s="2" t="n">
-        <v>45755.4665687426</v>
+        <v>45755.49764262247</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -3674,7 +3674,7 @@
         </is>
       </c>
       <c r="F75" s="2" t="n">
-        <v>45755.46656876175</v>
+        <v>45755.49764264091</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -3717,7 +3717,7 @@
         </is>
       </c>
       <c r="F76" s="2" t="n">
-        <v>45755.46656878325</v>
+        <v>45755.49764266142</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -3760,7 +3760,7 @@
         </is>
       </c>
       <c r="F77" s="2" t="n">
-        <v>45755.46656880165</v>
+        <v>45755.49764268007</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -3803,7 +3803,7 @@
         </is>
       </c>
       <c r="F78" s="2" t="n">
-        <v>45755.46656882529</v>
+        <v>45755.4976427026</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3846,7 +3846,7 @@
         </is>
       </c>
       <c r="F79" s="2" t="n">
-        <v>45755.46656884554</v>
+        <v>45755.49764272294</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3889,7 +3889,7 @@
         </is>
       </c>
       <c r="F80" s="2" t="n">
-        <v>45755.4665688641</v>
+        <v>45755.49764274171</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3932,7 +3932,7 @@
         </is>
       </c>
       <c r="F81" s="2" t="n">
-        <v>45755.46656888472</v>
+        <v>45755.49764276176</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -3975,7 +3975,7 @@
         </is>
       </c>
       <c r="F82" s="2" t="n">
-        <v>45755.46656890328</v>
+        <v>45755.49764278035</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -4018,7 +4018,7 @@
         </is>
       </c>
       <c r="F83" s="2" t="n">
-        <v>45755.46656892551</v>
+        <v>45755.49764280484</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -4061,7 +4061,7 @@
         </is>
       </c>
       <c r="F84" s="2" t="n">
-        <v>45755.46656894633</v>
+        <v>45755.49764282461</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -4104,7 +4104,7 @@
         </is>
       </c>
       <c r="F85" s="2" t="n">
-        <v>45755.46656896693</v>
+        <v>45755.49764284454</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>

</xml_diff>